<commit_message>
commit of Wiki Pages scraping & results file -- Gleixner
</commit_message>
<xml_diff>
--- a/research_data/Data to look at 09-09-20.xlsx
+++ b/research_data/Data to look at 09-09-20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gleix\Documents\CWRU_Education\Projects\Travel-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gleix\git\Travel-Project\research_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF70D3F-76AA-4EF5-AC26-EDF3D0A26588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813A9C39-EA1D-4A88-A6C0-686709902E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26790" yWindow="1125" windowWidth="23235" windowHeight="12555" xr2:uid="{FB74B22E-891F-4A1C-B53B-9BC1AFF088FC}"/>
+    <workbookView xWindow="8" yWindow="8" windowWidth="23025" windowHeight="12945" xr2:uid="{FB74B22E-891F-4A1C-B53B-9BC1AFF088FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,10 +352,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,7 +793,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -913,7 +920,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">

</xml_diff>